<commit_message>
Working on P4, to complete AB and Siege with cluster tests and graphs
</commit_message>
<xml_diff>
--- a/practica4/other files/resultados.xlsx
+++ b/practica4/other files/resultados.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="16">
   <si>
     <t>N TEST</t>
   </si>
@@ -80,7 +80,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,6 +94,13 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -147,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -155,22 +162,110 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="48">
+  <dxfs count="52">
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
+        <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -197,54 +292,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -262,47 +309,16 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="medium">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <top style="medium">
-          <color theme="1"/>
+          <color rgb="FF000000"/>
         </top>
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
       <border outline="0">
         <bottom style="medium">
-          <color theme="1"/>
+          <color rgb="FF000000"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="medium">
-          <color theme="1"/>
-        </top>
       </border>
     </dxf>
     <dxf>
@@ -347,16 +363,16 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="medium">
           <color rgb="FF000000"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="medium">
-          <color rgb="FF000000"/>
-        </top>
       </border>
     </dxf>
     <dxf>
@@ -384,6 +400,54 @@
     </dxf>
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -401,16 +465,28 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <top style="medium">
+          <color theme="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="medium">
-          <color rgb="FF000000"/>
+          <color theme="1"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="medium">
-          <color rgb="FF000000"/>
-        </top>
       </border>
     </dxf>
     <dxf>
@@ -455,16 +531,16 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <top style="medium">
+          <color theme="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="medium">
-          <color rgb="FF000000"/>
+          <color theme="1"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="medium">
-          <color rgb="FF000000"/>
-        </top>
       </border>
     </dxf>
     <dxf>
@@ -492,15 +568,34 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
+        <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="medium">
+          <color theme="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color theme="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -579,6 +674,13 @@
       </font>
     </dxf>
     <dxf>
+      <border outline="0">
+        <top style="medium">
+          <color theme="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -589,6 +691,13 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color theme="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -668,30 +777,28 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="medium">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <top style="medium">
           <color theme="1"/>
         </top>
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
       <border outline="0">
         <bottom style="medium">
           <color theme="1"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="medium">
-          <color theme="1"/>
-        </top>
       </border>
     </dxf>
     <dxf>
@@ -718,37 +825,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="medium">
-          <color theme="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
@@ -770,22 +846,1146 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="it-IT"/>
+              <a:t>OpenWebLoad</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Servidor Unico</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>OpenWebLoad!$B$14:$F$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2272.1260000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.33330000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.7801</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22730</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1418.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Granja Nginx</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>OpenWebLoad!$B$28:$F$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1176.2080000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.54180000000000006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.4745999999999988</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11775.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>806.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Granja Haproxy</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>OpenWebLoad!$B$42:$F$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1576.5419999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.46889999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.8617999999999988</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15771</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="444"/>
+        <c:overlap val="-90"/>
+        <c:axId val="2072460320"/>
+        <c:axId val="2072461408"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2072460320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2072461408"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2072461408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2072460320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="202">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabella2" displayName="Tabella2" ref="A3:D13" totalsRowShown="0">
   <autoFilter ref="A3:D13"/>
   <tableColumns count="4">
     <tableColumn id="1" name="N TEST"/>
-    <tableColumn id="2" name="TIME TAKEN" dataDxfId="47"/>
-    <tableColumn id="3" name="FAILED REQ" dataDxfId="46"/>
-    <tableColumn id="4" name="REQ PER SEC" dataDxfId="45"/>
+    <tableColumn id="2" name="TIME TAKEN" dataDxfId="51"/>
+    <tableColumn id="3" name="FAILED REQ" dataDxfId="50"/>
+    <tableColumn id="4" name="REQ PER SEC" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabella357" displayName="Tabella357" ref="A17:D27" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31" headerRowBorderDxfId="39" tableBorderDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabella357" displayName="Tabella357" ref="A17:D27" totalsRowShown="0" headerRowDxfId="48" dataDxfId="46" headerRowBorderDxfId="47" tableBorderDxfId="45">
   <autoFilter ref="A17:D27"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="N TEST" dataDxfId="44"/>
+    <tableColumn id="2" name="TIME TAKEN" dataDxfId="43"/>
+    <tableColumn id="3" name="FAILED REQ" dataDxfId="42"/>
+    <tableColumn id="4" name="REQ PER SEC" dataDxfId="41"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabella368" displayName="Tabella368" ref="A31:D41" totalsRowShown="0" headerRowDxfId="40" dataDxfId="38" headerRowBorderDxfId="39" tableBorderDxfId="37">
+  <autoFilter ref="A31:D41"/>
   <tableColumns count="4">
     <tableColumn id="1" name="N TEST" dataDxfId="36"/>
     <tableColumn id="2" name="TIME TAKEN" dataDxfId="35"/>
@@ -796,24 +1996,11 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabella368" displayName="Tabella368" ref="A31:D41" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25" headerRowBorderDxfId="37" tableBorderDxfId="38">
-  <autoFilter ref="A31:D41"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="N TEST" dataDxfId="30"/>
-    <tableColumn id="2" name="TIME TAKEN" dataDxfId="29"/>
-    <tableColumn id="3" name="FAILED REQ" dataDxfId="28"/>
-    <tableColumn id="4" name="REQ PER SEC" dataDxfId="27"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabella3" displayName="Tabella3" ref="A3:E13" totalsRowShown="0" headerRowDxfId="41" headerRowBorderDxfId="43" tableBorderDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabella3" displayName="Tabella3" ref="A3:E13" totalsRowShown="0" headerRowDxfId="32" headerRowBorderDxfId="31" tableBorderDxfId="30">
   <autoFilter ref="A3:E13"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="N TEST" dataDxfId="42"/>
+    <tableColumn id="1" name="N TEST" dataDxfId="29"/>
     <tableColumn id="2" name="Availability"/>
     <tableColumn id="3" name="Elapsed time"/>
     <tableColumn id="4" name="Response time"/>
@@ -824,10 +2011,10 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabella312" displayName="Tabella312" ref="A17:E27" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="10" tableBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabella312" displayName="Tabella312" ref="A17:E27" totalsRowShown="0" headerRowDxfId="28" headerRowBorderDxfId="27" tableBorderDxfId="26">
   <autoFilter ref="A17:E27"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="N TEST" dataDxfId="9"/>
+    <tableColumn id="1" name="N TEST" dataDxfId="25"/>
     <tableColumn id="2" name="Availability"/>
     <tableColumn id="3" name="Elapsed time"/>
     <tableColumn id="4" name="Response time"/>
@@ -838,55 +2025,87 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tabella313" displayName="Tabella313" ref="A31:E41" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="7" tableBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tabella313" displayName="Tabella313" ref="A31:E41" totalsRowShown="0" headerRowDxfId="24" dataDxfId="22" headerRowBorderDxfId="23" tableBorderDxfId="21">
   <autoFilter ref="A31:E41"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="N TEST" dataDxfId="6"/>
-    <tableColumn id="2" name="Availability" dataDxfId="5"/>
-    <tableColumn id="3" name="Elapsed time" dataDxfId="4"/>
-    <tableColumn id="4" name="Response time" dataDxfId="3"/>
-    <tableColumn id="5" name="Transaction rate" dataDxfId="2"/>
+    <tableColumn id="1" name="N TEST" dataDxfId="20"/>
+    <tableColumn id="2" name="Availability" dataDxfId="19"/>
+    <tableColumn id="3" name="Elapsed time" dataDxfId="18"/>
+    <tableColumn id="4" name="Response time" dataDxfId="17"/>
+    <tableColumn id="5" name="Transaction rate" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabella39" displayName="Tabella39" ref="A3:F13" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="22" tableBorderDxfId="23">
-  <autoFilter ref="A3:F13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabella39" displayName="Tabella39" ref="A3:F14" totalsRowCount="1" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13">
+  <autoFilter ref="A3:F14"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="N TEST" dataDxfId="21"/>
-    <tableColumn id="2" name="Total TPS"/>
-    <tableColumn id="3" name="Avg Response Time"/>
-    <tableColumn id="4" name="Max Response Time"/>
-    <tableColumn id="5" name="Total Requests"/>
-    <tableColumn id="6" name="Total Errors"/>
+    <tableColumn id="1" name="N TEST" dataDxfId="12" totalsRowDxfId="3"/>
+    <tableColumn id="2" name="Total TPS" totalsRowFunction="average"/>
+    <tableColumn id="3" name="Avg Response Time" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(101,C4:C13)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" name="Max Response Time" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(101,D4:D13)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="5" name="Total Requests" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(101,E4:E13)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="6" name="Total Errors" totalsRowFunction="custom" totalsRowDxfId="2">
+      <totalsRowFormula>SUBTOTAL(101,F4:F13)</totalsRowFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabella3510" displayName="Tabella3510" ref="A17:D27" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="18" tableBorderDxfId="19">
-  <autoFilter ref="A17:D27"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="N TEST" dataDxfId="17"/>
-    <tableColumn id="2" name="TIME TAKEN"/>
-    <tableColumn id="3" name="FAILED REQ"/>
-    <tableColumn id="4" name="REQ PER SEC"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabella3510" displayName="Tabella3510" ref="A17:F28" totalsRowCount="1" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9">
+  <autoFilter ref="A17:F28"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="N TEST" dataDxfId="8" totalsRowDxfId="1"/>
+    <tableColumn id="2" name="Total TPS" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(101,B18:B27)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="3" name="Avg Response Time" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(101,C18:C27)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" name="Max Response Time" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(101,D18:D27)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="5" name="Total Requests" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(101,E18:E27)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="6" name="Total Errors" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(101,F18:F27)</totalsRowFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabella3611" displayName="Tabella3611" ref="A31:D41" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="14" tableBorderDxfId="15">
-  <autoFilter ref="A31:D41"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="N TEST" dataDxfId="13"/>
-    <tableColumn id="2" name="TIME TAKEN"/>
-    <tableColumn id="3" name="FAILED REQ"/>
-    <tableColumn id="4" name="REQ PER SEC"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabella3611" displayName="Tabella3611" ref="A31:F42" totalsRowCount="1" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5">
+  <autoFilter ref="A31:F42"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="N TEST" dataDxfId="4" totalsRowDxfId="0"/>
+    <tableColumn id="2" name="Total TPS" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(101,B32:B41)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="3" name="Avg Response Time" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(101,C32:C41)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" name="Max Response Time" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(101,D32:D41)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="5" name="Total Requests" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(101,E32:E41)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="6" name="Total Errors" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(101,F32:F41)</totalsRowFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1968,10 +3187,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F41"/>
+  <dimension ref="A2:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2207,152 +3426,532 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F14" s="1"/>
+      <c r="A14" s="1"/>
+      <c r="B14">
+        <f>SUBTOTAL(101,Tabella39[Total TPS])</f>
+        <v>2272.1260000000002</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14:F14" si="0">SUBTOTAL(101,C4:C13)</f>
+        <v>0.33330000000000004</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>7.7801</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>22730</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="0"/>
+        <v>1418.2</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>1204.18</v>
+      </c>
+      <c r="C18">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="D18">
+        <v>9.5289999999999999</v>
+      </c>
+      <c r="E18">
+        <v>12043</v>
+      </c>
+      <c r="F18">
+        <v>1217</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>1077.69</v>
+      </c>
+      <c r="C19">
+        <v>0.57399999999999995</v>
+      </c>
+      <c r="D19">
+        <v>9.5920000000000005</v>
+      </c>
+      <c r="E19">
+        <v>10778</v>
+      </c>
+      <c r="F19">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>1141.06</v>
+      </c>
+      <c r="C20">
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="D20">
+        <v>9.516</v>
+      </c>
+      <c r="E20">
+        <v>11414</v>
+      </c>
+      <c r="F20">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>1128.57</v>
+      </c>
+      <c r="C21">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="D21">
+        <v>8.7509999999999994</v>
+      </c>
+      <c r="E21">
+        <v>11288</v>
+      </c>
+      <c r="F21">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>1127.5899999999999</v>
+      </c>
+      <c r="C22">
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="D22">
+        <v>9.6579999999999995</v>
+      </c>
+      <c r="E22">
+        <v>11277</v>
+      </c>
+      <c r="F22">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>1268.1300000000001</v>
+      </c>
+      <c r="C23">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="D23">
+        <v>9.5419999999999998</v>
+      </c>
+      <c r="E23">
+        <v>12784</v>
+      </c>
+      <c r="F23">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>1268.79</v>
+      </c>
+      <c r="C24">
+        <v>0.59799999999999998</v>
+      </c>
+      <c r="D24">
+        <v>9.5359999999999996</v>
+      </c>
+      <c r="E24">
+        <v>12693</v>
+      </c>
+      <c r="F24">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>1171.05</v>
+      </c>
+      <c r="C25">
+        <v>0.55200000000000005</v>
+      </c>
+      <c r="D25">
+        <v>9.5239999999999991</v>
+      </c>
+      <c r="E25">
+        <v>11714</v>
+      </c>
+      <c r="F25">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>1201.24</v>
+      </c>
+      <c r="C26">
+        <v>0.498</v>
+      </c>
+      <c r="D26">
+        <v>9.5809999999999995</v>
+      </c>
+      <c r="E26">
+        <v>12016</v>
+      </c>
+      <c r="F26">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>1173.78</v>
+      </c>
+      <c r="C27">
+        <v>0.498</v>
+      </c>
+      <c r="D27">
+        <v>9.5169999999999995</v>
+      </c>
+      <c r="E27">
+        <v>11746</v>
+      </c>
+      <c r="F27">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28">
+        <f t="shared" ref="B28:F28" si="1">SUBTOTAL(101,B18:B27)</f>
+        <v>1176.2080000000001</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="1"/>
+        <v>0.54180000000000006</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>9.4745999999999988</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="1"/>
+        <v>11775.3</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>806.6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>1683.72</v>
+      </c>
+      <c r="C32">
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="D32">
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="E32">
+        <v>16849</v>
+      </c>
+      <c r="F32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>1528.55</v>
+      </c>
+      <c r="C33">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="D33">
+        <v>8.9390000000000001</v>
+      </c>
+      <c r="E33">
+        <v>15287</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>1531.89</v>
+      </c>
+      <c r="C34">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="D34">
+        <v>8.9440000000000008</v>
+      </c>
+      <c r="E34">
+        <v>15325</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>1533.78</v>
+      </c>
+      <c r="C35">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="D35">
+        <v>8.9489999999999998</v>
+      </c>
+      <c r="E35">
+        <v>15347</v>
+      </c>
+      <c r="F35">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>1521.5</v>
+      </c>
+      <c r="C36">
+        <v>0.45900000000000002</v>
+      </c>
+      <c r="D36">
+        <v>8.9969999999999999</v>
+      </c>
+      <c r="E36">
+        <v>15218</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>1682.9</v>
+      </c>
+      <c r="C37">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="D37">
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="E37">
+        <v>16834</v>
+      </c>
+      <c r="F37">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>1514.9</v>
+      </c>
+      <c r="C38">
+        <v>0.441</v>
+      </c>
+      <c r="D38">
+        <v>8.08</v>
+      </c>
+      <c r="E38">
+        <v>15152</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>1531.09</v>
+      </c>
+      <c r="C39">
+        <v>0.44600000000000001</v>
+      </c>
+      <c r="D39">
+        <v>8.9339999999999993</v>
+      </c>
+      <c r="E39">
+        <v>15317</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40">
+        <v>1518.05</v>
+      </c>
+      <c r="C40">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="D40">
+        <v>8.9480000000000004</v>
+      </c>
+      <c r="E40">
+        <v>15182</v>
+      </c>
+      <c r="F40">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>10</v>
       </c>
+      <c r="B41">
+        <v>1719.04</v>
+      </c>
+      <c r="C41">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="D41">
+        <v>8.9269999999999996</v>
+      </c>
+      <c r="E41">
+        <v>17199</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42">
+        <f t="shared" ref="B42:F42" si="2">SUBTOTAL(101,B32:B41)</f>
+        <v>1576.5419999999999</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="2"/>
+        <v>0.46889999999999998</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="2"/>
+        <v>8.8617999999999988</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="2"/>
+        <v>15771</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="2"/>
+        <v>15.1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="3">
-    <tablePart r:id="rId1"/>
-    <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>